<commit_message>
Rev'd board design and schematic to utilize smaller-footprint 8MHz crystal resonators.
</commit_message>
<xml_diff>
--- a/Hardware/MSP430AFE253_Demo_Board_BOM.xlsx
+++ b/Hardware/MSP430AFE253_Demo_Board_BOM.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="203">
   <si>
     <t>Mfg</t>
   </si>
@@ -591,9 +591,6 @@
     <t>QFN-24_0.65MM</t>
   </si>
   <si>
-    <t>USB_MINI_B_RA_SMT</t>
-  </si>
-  <si>
     <t>TB_100MIL_1R8P_PTH</t>
   </si>
   <si>
@@ -646,6 +643,27 @@
   </si>
   <si>
     <t>Murata</t>
+  </si>
+  <si>
+    <t>USB_MINI_AB_RA_SMT</t>
+  </si>
+  <si>
+    <t>490-1195-1-ND</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>CSTCE8M00G55-R0</t>
+  </si>
+  <si>
+    <t>CER RESONATOR 8.00MHZ SMD</t>
+  </si>
+  <si>
+    <t>MCU Clock, USB-to-Serial Converter</t>
+  </si>
+  <si>
+    <t>CER_RES_1.2MM_SMT</t>
   </si>
 </sst>
 </file>
@@ -694,7 +712,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -717,11 +735,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -751,6 +780,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2286,10 +2316,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,7 +2408,7 @@
         <v>1.68</v>
       </c>
       <c r="K2" s="7">
-        <f t="shared" ref="K2:K24" si="0">J2*G2</f>
+        <f t="shared" ref="K2:K25" si="0">J2*G2</f>
         <v>1.68</v>
       </c>
       <c r="L2" s="6" t="s">
@@ -2402,7 +2432,7 @@
         <v>149</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>178</v>
+        <v>196</v>
       </c>
       <c r="G3" s="5">
         <v>1</v>
@@ -2441,7 +2471,7 @@
         <v>150</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G4" s="5">
         <v>1</v>
@@ -2480,7 +2510,7 @@
         <v>154</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G5" s="5">
         <v>2</v>
@@ -2519,7 +2549,7 @@
         <v>147</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
@@ -2558,7 +2588,7 @@
         <v>167</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -2595,7 +2625,7 @@
         <v>162</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G8" s="5">
         <v>6</v>
@@ -2632,7 +2662,7 @@
         <v>163</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G9" s="5">
         <v>2</v>
@@ -2669,7 +2699,7 @@
         <v>166</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G10" s="5">
         <v>4</v>
@@ -2706,7 +2736,7 @@
         <v>165</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G11" s="5">
         <v>2</v>
@@ -2743,7 +2773,7 @@
         <v>164</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
@@ -2780,7 +2810,7 @@
         <v>160</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G13" s="5">
         <v>3</v>
@@ -2819,7 +2849,7 @@
         <v>158</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G14" s="5">
         <v>1</v>
@@ -2858,7 +2888,7 @@
         <v>156</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G15" s="5">
         <v>1</v>
@@ -2897,7 +2927,7 @@
         <v>157</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G16" s="5">
         <v>1</v>
@@ -2926,7 +2956,7 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E17" s="10" t="s">
         <v>159</v>
@@ -2958,7 +2988,7 @@
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>151</v>
@@ -2990,7 +3020,7 @@
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>173</v>
@@ -3032,7 +3062,7 @@
         <v>152</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G20" s="5">
         <v>1</v>
@@ -3071,7 +3101,7 @@
         <v>153</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G21" s="5">
         <v>1</v>
@@ -3098,28 +3128,28 @@
         <v>23</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="E22" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="G22" s="5">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="G22" s="5">
-        <v>0</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="J22" s="7">
         <v>0.48</v>
@@ -3128,7 +3158,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L22" s="6"/>
+      <c r="L22" s="6" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -3147,7 +3179,7 @@
         <v>161</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G23" s="5">
         <v>7</v>
@@ -3176,7 +3208,7 @@
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>155</v>
@@ -3199,6 +3231,45 @@
       </c>
       <c r="L24" s="6" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>36</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="K25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The Freescale USB-to-Serial IC seems to be obsolee.  This is a baseline check-in before changing to the FTDI FT230XQ.
</commit_message>
<xml_diff>
--- a/Hardware/MSP430AFE253_Demo_Board_BOM.xlsx
+++ b/Hardware/MSP430AFE253_Demo_Board_BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="15" windowWidth="15720" windowHeight="12810" tabRatio="701" activeTab="1"/>
+    <workbookView xWindow="3240" yWindow="15" windowWidth="15720" windowHeight="12810" tabRatio="701"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Component Choices" sheetId="1" r:id="rId1"/>
@@ -712,7 +712,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -735,22 +735,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -780,7 +769,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1084,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,8 +2306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,16 +3222,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="5">
         <v>36</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="8" t="s">
         <v>200</v>
       </c>
       <c r="E25" s="10" t="s">
@@ -3252,16 +3240,16 @@
       <c r="F25" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G25" s="1">
-        <v>0</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="15" t="s">
+      <c r="G25" s="5">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="7">
         <v>0.46</v>
       </c>
       <c r="K25" s="7">

</xml_diff>